<commit_message>
Personal report, over timesheet (not yet completed)
</commit_message>
<xml_diff>
--- a/N17/Legacy/man/timesheets/timesheet_matt.xlsx
+++ b/N17/Legacy/man/timesheets/timesheet_matt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,33 @@
   </si>
   <si>
     <t>Group 17</t>
+  </si>
+  <si>
+    <t>Testing in work week</t>
+  </si>
+  <si>
+    <t>Testing in work week/also completing test documentation</t>
+  </si>
+  <si>
+    <t>Final testing</t>
+  </si>
+  <si>
+    <t>Testing in work week/also imrpoving on design documentation</t>
+  </si>
+  <si>
+    <t>Completing my personal report</t>
+  </si>
+  <si>
+    <t>Completing the change in control forms</t>
+  </si>
+  <si>
+    <t>Complete the timesheet documentation</t>
+  </si>
+  <si>
+    <t>Comleting my timesheet</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -397,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +464,7 @@
         <v>41201</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -448,7 +475,7 @@
         <v>41204</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -470,7 +497,7 @@
         <v>41208</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -619,12 +646,128 @@
         <v>6</v>
       </c>
     </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>41302</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>41303</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>41304</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>41305</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>41306</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>41312</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>41317</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>41317</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>41317</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>41317</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
       <c r="K29" t="s">
         <v>12</v>
       </c>
       <c r="M29" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>